<commit_message>
clean up predefined age group definitions
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/agegroups/FHQ-AgeGroups_fr_CA.xlsx
+++ b/owlcms/src/main/resources/agegroups/FHQ-AgeGroups_fr_CA.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\agegroups\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\local\agegroups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63185A53-D3A5-49B7-B09A-3B9A0BF93F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16D41ED-4602-4FF5-A713-38D41C9F5125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="1335" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2745" yWindow="1065" windowWidth="21600" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AgeGroups" sheetId="2" r:id="rId1"/>
+    <sheet name="BW Categories" sheetId="1" r:id="rId1"/>
+    <sheet name="AgeGroups" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="175">
   <si>
     <t>code</t>
   </si>
@@ -43,15 +44,33 @@
     <t>#default bw categories</t>
   </si>
   <si>
+    <t>max_bw</t>
+  </si>
+  <si>
+    <t>WR_SR</t>
+  </si>
+  <si>
+    <t>WR_JR</t>
+  </si>
+  <si>
+    <t>WR_YTH</t>
+  </si>
+  <si>
     <t>M35</t>
   </si>
   <si>
     <t>M</t>
   </si>
   <si>
+    <t>https://en.wikipedia.org/wiki/List_of_world_records_in_Olympic_weightlifting#Men</t>
+  </si>
+  <si>
     <t>M40</t>
   </si>
   <si>
+    <t>https://en.wikipedia.org/wiki/List_of_junior_world_records_in_Olympic_weightlifting#Men</t>
+  </si>
+  <si>
     <t>M45</t>
   </si>
   <si>
@@ -88,6 +107,9 @@
     <t>M999</t>
   </si>
   <si>
+    <t>M999 is always used as the last category in an age group</t>
+  </si>
+  <si>
     <t>F35</t>
   </si>
   <si>
@@ -124,9 +146,6 @@
     <t>F71</t>
   </si>
   <si>
-    <t>U15</t>
-  </si>
-  <si>
     <t>F76</t>
   </si>
   <si>
@@ -163,6 +182,9 @@
     <t>F75</t>
   </si>
   <si>
+    <t>F999 is always used as the last category in an age group</t>
+  </si>
+  <si>
     <t>F70+</t>
   </si>
   <si>
@@ -202,9 +224,6 @@
     <t>F80+</t>
   </si>
   <si>
-    <t>U12</t>
-  </si>
-  <si>
     <t>F40 35</t>
   </si>
   <si>
@@ -316,111 +335,21 @@
     <t>M45 49</t>
   </si>
   <si>
-    <t>M49 55</t>
-  </si>
-  <si>
-    <t>M55 59</t>
-  </si>
-  <si>
-    <t>M61 65</t>
-  </si>
-  <si>
-    <t>M67 71</t>
-  </si>
-  <si>
-    <t>M73 79</t>
-  </si>
-  <si>
-    <t>M81 87</t>
-  </si>
-  <si>
-    <t>M999 91</t>
-  </si>
-  <si>
-    <t>F45 45</t>
-  </si>
-  <si>
     <t>F49 49</t>
   </si>
   <si>
-    <t>F55 55</t>
-  </si>
-  <si>
-    <t>F59 59</t>
-  </si>
-  <si>
-    <t>F64 64</t>
-  </si>
-  <si>
     <t>F71 71</t>
   </si>
   <si>
-    <t>F76 76</t>
-  </si>
-  <si>
-    <t>F999 80</t>
-  </si>
-  <si>
-    <t>F45 110</t>
-  </si>
-  <si>
-    <t>F49 131</t>
-  </si>
-  <si>
-    <t>F55 141</t>
-  </si>
-  <si>
-    <t>F59 152</t>
-  </si>
-  <si>
-    <t>F64 159</t>
-  </si>
-  <si>
     <t>F71 160</t>
   </si>
   <si>
     <t>F76 167</t>
   </si>
   <si>
-    <t>F81 168</t>
-  </si>
-  <si>
-    <t>F87 170</t>
-  </si>
-  <si>
-    <t>F999 183</t>
-  </si>
-  <si>
-    <t>M999 283</t>
-  </si>
-  <si>
-    <t>M55 176</t>
-  </si>
-  <si>
     <t>M61 198</t>
   </si>
   <si>
-    <t>M67 215</t>
-  </si>
-  <si>
-    <t>M73 229</t>
-  </si>
-  <si>
-    <t>M81 241</t>
-  </si>
-  <si>
-    <t>M89 246</t>
-  </si>
-  <si>
-    <t>M96 261</t>
-  </si>
-  <si>
-    <t>M102 263</t>
-  </si>
-  <si>
-    <t>M109 266</t>
-  </si>
-  <si>
     <t>CU</t>
   </si>
   <si>
@@ -479,13 +408,151 @@
   </si>
   <si>
     <t>OPEN</t>
+  </si>
+  <si>
+    <t>Mini</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>F40 36</t>
+  </si>
+  <si>
+    <t>F45 41</t>
+  </si>
+  <si>
+    <t>F55 53</t>
+  </si>
+  <si>
+    <t>F59 57</t>
+  </si>
+  <si>
+    <t>F64 60</t>
+  </si>
+  <si>
+    <t>F71 63</t>
+  </si>
+  <si>
+    <t>F999 67</t>
+  </si>
+  <si>
+    <t>M40 36</t>
+  </si>
+  <si>
+    <t>M45 41</t>
+  </si>
+  <si>
+    <t>M49 49</t>
+  </si>
+  <si>
+    <t>M55 53</t>
+  </si>
+  <si>
+    <t>M61 59</t>
+  </si>
+  <si>
+    <t>M67 64</t>
+  </si>
+  <si>
+    <t>F45 46</t>
+  </si>
+  <si>
+    <t>F49 54</t>
+  </si>
+  <si>
+    <t>F55 58</t>
+  </si>
+  <si>
+    <t>F59 63</t>
+  </si>
+  <si>
+    <t>F64 67</t>
+  </si>
+  <si>
+    <t>F76 75</t>
+  </si>
+  <si>
+    <t>F999 79</t>
+  </si>
+  <si>
+    <t>M49 54</t>
+  </si>
+  <si>
+    <t>M55 60</t>
+  </si>
+  <si>
+    <t>M61 67</t>
+  </si>
+  <si>
+    <t>M67 72</t>
+  </si>
+  <si>
+    <t>M73 78</t>
+  </si>
+  <si>
+    <t>M81 84</t>
+  </si>
+  <si>
+    <t>M999 90</t>
+  </si>
+  <si>
+    <t>F45 118</t>
+  </si>
+  <si>
+    <t>F49 126</t>
+  </si>
+  <si>
+    <t>F55 137</t>
+  </si>
+  <si>
+    <t>F59 144</t>
+  </si>
+  <si>
+    <t>F64 151</t>
+  </si>
+  <si>
+    <t>F81 172</t>
+  </si>
+  <si>
+    <t>F87 177</t>
+  </si>
+  <si>
+    <t>F999 186</t>
+  </si>
+  <si>
+    <t>M55 182</t>
+  </si>
+  <si>
+    <t>M67 210</t>
+  </si>
+  <si>
+    <t>M73 223</t>
+  </si>
+  <si>
+    <t>M81 237</t>
+  </si>
+  <si>
+    <t>M89 249</t>
+  </si>
+  <si>
+    <t>M96 257</t>
+  </si>
+  <si>
+    <t>M102 265</t>
+  </si>
+  <si>
+    <t>M109 271</t>
+  </si>
+  <si>
+    <t>M999 284</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -501,6 +568,20 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -537,18 +618,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -764,6 +847,542 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:H27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4">
+        <v>35</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="H2" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="H3" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4">
+        <v>45</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4">
+        <v>49</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="4">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4">
+        <v>55</v>
+      </c>
+      <c r="D6" s="4">
+        <v>294</v>
+      </c>
+      <c r="E6" s="4">
+        <v>264</v>
+      </c>
+      <c r="F6" s="4">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="4">
+        <v>61</v>
+      </c>
+      <c r="D7" s="4">
+        <v>318</v>
+      </c>
+      <c r="E7" s="4">
+        <v>293</v>
+      </c>
+      <c r="F7" s="4">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4">
+        <v>67</v>
+      </c>
+      <c r="D8" s="4">
+        <v>339</v>
+      </c>
+      <c r="E8" s="4">
+        <v>328</v>
+      </c>
+      <c r="F8" s="4">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="4">
+        <v>73</v>
+      </c>
+      <c r="D9" s="4">
+        <v>363</v>
+      </c>
+      <c r="E9" s="4">
+        <v>347</v>
+      </c>
+      <c r="F9" s="4">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="4">
+        <v>81</v>
+      </c>
+      <c r="D10" s="4">
+        <v>378</v>
+      </c>
+      <c r="E10" s="4">
+        <v>372</v>
+      </c>
+      <c r="F10" s="4">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="4">
+        <v>89</v>
+      </c>
+      <c r="D11" s="4">
+        <v>387</v>
+      </c>
+      <c r="E11" s="4">
+        <v>371</v>
+      </c>
+      <c r="F11" s="4">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="4">
+        <v>96</v>
+      </c>
+      <c r="D12" s="4">
+        <v>416</v>
+      </c>
+      <c r="E12" s="4">
+        <v>397</v>
+      </c>
+      <c r="F12" s="4">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="4">
+        <v>102</v>
+      </c>
+      <c r="D13" s="4">
+        <v>412</v>
+      </c>
+      <c r="E13" s="4">
+        <v>392</v>
+      </c>
+      <c r="F13" s="4">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="4">
+        <v>109</v>
+      </c>
+      <c r="D14" s="4">
+        <v>435</v>
+      </c>
+      <c r="E14" s="4">
+        <v>417</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4">
+        <v>999</v>
+      </c>
+      <c r="D15" s="4">
+        <v>484</v>
+      </c>
+      <c r="E15" s="4">
+        <v>432</v>
+      </c>
+      <c r="F15" s="4">
+        <v>396</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="4">
+        <v>35</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="4">
+        <v>40</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="4">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="4">
+        <v>45</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="4">
+        <v>179</v>
+      </c>
+      <c r="F18" s="4">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="4">
+        <v>49</v>
+      </c>
+      <c r="D19" s="4">
+        <v>210</v>
+      </c>
+      <c r="E19" s="4">
+        <v>206</v>
+      </c>
+      <c r="F19" s="4">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="4">
+        <v>55</v>
+      </c>
+      <c r="D20" s="4">
+        <v>232</v>
+      </c>
+      <c r="E20" s="4">
+        <v>211</v>
+      </c>
+      <c r="F20" s="4">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="4">
+        <v>59</v>
+      </c>
+      <c r="D21" s="4">
+        <v>237</v>
+      </c>
+      <c r="E21" s="4">
+        <v>228</v>
+      </c>
+      <c r="F21" s="4">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="4">
+        <v>64</v>
+      </c>
+      <c r="D22" s="4">
+        <v>254</v>
+      </c>
+      <c r="E22" s="4">
+        <v>240</v>
+      </c>
+      <c r="F22" s="4">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="4">
+        <v>71</v>
+      </c>
+      <c r="D23" s="4">
+        <v>267</v>
+      </c>
+      <c r="E23" s="4">
+        <v>252</v>
+      </c>
+      <c r="F23" s="4">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="4">
+        <v>76</v>
+      </c>
+      <c r="D24" s="4">
+        <v>274</v>
+      </c>
+      <c r="E24" s="4">
+        <v>259</v>
+      </c>
+      <c r="F24" s="4">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="4">
+        <v>81</v>
+      </c>
+      <c r="D25" s="4">
+        <v>283</v>
+      </c>
+      <c r="E25" s="4">
+        <v>260</v>
+      </c>
+      <c r="F25" s="4">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="4">
+        <v>87</v>
+      </c>
+      <c r="D26" s="4">
+        <v>294</v>
+      </c>
+      <c r="E26" s="4">
+        <v>269</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="4">
+        <v>999</v>
+      </c>
+      <c r="D27" s="4">
+        <v>330</v>
+      </c>
+      <c r="E27" s="4">
+        <v>332</v>
+      </c>
+      <c r="F27" s="4">
+        <v>255</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" location="Men" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H3" r:id="rId2" location="Men" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -771,7 +1390,7 @@
   <dimension ref="A1:U46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="C44" sqref="C44:E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -799,45 +1418,45 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3">
+        <v>30</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
         <v>10</v>
       </c>
-      <c r="G2" s="5" t="b">
+      <c r="G2" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -855,48 +1474,48 @@
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>60</v>
+        <v>129</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="3">
+        <v>30</v>
+      </c>
+      <c r="E3" s="4">
+        <v>9</v>
+      </c>
+      <c r="F3" s="4">
         <v>11</v>
       </c>
-      <c r="F3" s="3">
-        <v>12</v>
-      </c>
-      <c r="G3" s="5" t="b">
-        <v>0</v>
+      <c r="G3" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>63</v>
+        <v>132</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>65</v>
+        <v>133</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>66</v>
+        <v>134</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>67</v>
+        <v>135</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>69</v>
+        <v>137</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -906,48 +1525,48 @@
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="3">
+        <v>30</v>
+      </c>
+      <c r="E4" s="4">
         <v>11</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="4">
         <v>13</v>
       </c>
-      <c r="G4" s="5" t="b">
+      <c r="G4" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -957,49 +1576,49 @@
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>130</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="3">
-        <v>11</v>
-      </c>
-      <c r="F5" s="3">
+        <v>30</v>
+      </c>
+      <c r="E5" s="4">
+        <v>12</v>
+      </c>
+      <c r="F5" s="4">
         <v>15</v>
       </c>
-      <c r="G5" s="5" t="b">
-        <v>0</v>
+      <c r="G5" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="P5" s="1" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>112</v>
+        <v>150</v>
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -1008,52 +1627,52 @@
     </row>
     <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="3">
-        <v>12</v>
-      </c>
-      <c r="F6" s="3">
+        <v>30</v>
+      </c>
+      <c r="E6" s="4">
+        <v>12</v>
+      </c>
+      <c r="F6" s="4">
         <v>17</v>
       </c>
-      <c r="G6" s="5" t="b">
+      <c r="G6" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="O6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R6" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
@@ -1061,49 +1680,49 @@
     </row>
     <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="3">
-        <v>12</v>
-      </c>
-      <c r="F7" s="3">
+        <v>30</v>
+      </c>
+      <c r="E7" s="4">
+        <v>12</v>
+      </c>
+      <c r="F7" s="4">
         <v>18</v>
       </c>
-      <c r="G7" s="5" t="b">
+      <c r="G7" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -1112,769 +1731,769 @@
     </row>
     <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="3">
+        <v>30</v>
+      </c>
+      <c r="E8" s="4">
         <v>17</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="4">
         <v>30</v>
       </c>
-      <c r="G8" s="5" t="b">
+      <c r="G8" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="3">
         <v>30</v>
       </c>
-      <c r="F9" s="3">
+      <c r="E9" s="4">
+        <v>30</v>
+      </c>
+      <c r="F9" s="4">
         <v>34</v>
       </c>
-      <c r="G9" s="5" t="b">
+      <c r="G9" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="O9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S9" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
     <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="3">
+        <v>30</v>
+      </c>
+      <c r="E10" s="4">
         <v>35</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="4">
         <v>39</v>
       </c>
-      <c r="G10" s="5" t="b">
+      <c r="G10" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="O10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S10" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
     </row>
     <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="3">
+        <v>30</v>
+      </c>
+      <c r="E11" s="4">
         <v>40</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="4">
         <v>44</v>
       </c>
-      <c r="G11" s="5" t="b">
+      <c r="G11" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="O11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S11" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
     </row>
     <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="3">
+        <v>30</v>
+      </c>
+      <c r="E12" s="4">
         <v>45</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="4">
         <v>49</v>
       </c>
-      <c r="G12" s="5" t="b">
+      <c r="G12" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="O12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S12" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
     </row>
     <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="3">
+        <v>30</v>
+      </c>
+      <c r="E13" s="4">
         <v>50</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="4">
         <v>54</v>
       </c>
-      <c r="G13" s="5" t="b">
+      <c r="G13" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="O13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S13" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
     </row>
     <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="3">
+        <v>30</v>
+      </c>
+      <c r="E14" s="4">
         <v>55</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="4">
         <v>59</v>
       </c>
-      <c r="G14" s="5" t="b">
+      <c r="G14" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="O14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S14" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
     </row>
     <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="3">
+        <v>30</v>
+      </c>
+      <c r="E15" s="4">
         <v>60</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="4">
         <v>64</v>
       </c>
-      <c r="G15" s="5" t="b">
+      <c r="G15" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="O15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S15" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
     </row>
     <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="3">
+        <v>30</v>
+      </c>
+      <c r="E16" s="4">
         <v>65</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="4">
         <v>69</v>
       </c>
-      <c r="G16" s="5" t="b">
+      <c r="G16" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="O16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S16" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S16" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
     </row>
     <row r="17" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="3">
+        <v>30</v>
+      </c>
+      <c r="E17" s="4">
         <v>70</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="4">
         <v>74</v>
       </c>
-      <c r="G17" s="5" t="b">
+      <c r="G17" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="O17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S17" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S17" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
     </row>
     <row r="18" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="3">
+        <v>30</v>
+      </c>
+      <c r="E18" s="4">
         <v>75</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="4">
         <v>79</v>
       </c>
-      <c r="G18" s="5" t="b">
+      <c r="G18" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="O18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S18" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S18" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
     </row>
     <row r="19" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="3">
+        <v>30</v>
+      </c>
+      <c r="E19" s="4">
         <v>80</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="4">
         <v>999</v>
       </c>
-      <c r="G19" s="5" t="b">
+      <c r="G19" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="O19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S19" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
     </row>
     <row r="20" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="3">
+        <v>30</v>
+      </c>
+      <c r="E20" s="4">
         <v>70</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="4">
         <v>999</v>
       </c>
-      <c r="G20" s="5" t="b">
+      <c r="G20" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="O20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S20" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
     </row>
     <row r="21" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" s="3">
+        <v>30</v>
+      </c>
+      <c r="E21" s="4">
         <v>13</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="4">
         <v>17</v>
       </c>
-      <c r="G21" s="5" t="b">
+      <c r="G21" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="O21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R21" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
@@ -1882,195 +2501,195 @@
     </row>
     <row r="22" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="3">
+        <v>30</v>
+      </c>
+      <c r="E22" s="4">
         <v>15</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="4">
         <v>20</v>
       </c>
-      <c r="G22" s="5" t="b">
+      <c r="G22" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
     </row>
     <row r="23" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" s="3">
+        <v>30</v>
+      </c>
+      <c r="E23" s="4">
         <v>15</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="4">
         <v>999</v>
       </c>
-      <c r="G23" s="5" t="b">
+      <c r="G23" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1" t="s">
-        <v>113</v>
+        <v>158</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>114</v>
+        <v>159</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>116</v>
+        <v>161</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>117</v>
+        <v>162</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>120</v>
+        <v>163</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>121</v>
+        <v>164</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>122</v>
+        <v>165</v>
       </c>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
     </row>
     <row r="24" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="3">
-        <v>0</v>
-      </c>
-      <c r="F24" s="3">
+        <v>30</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4">
         <v>999</v>
       </c>
-      <c r="G24" s="5" t="b">
-        <v>1</v>
+      <c r="G24" s="7" t="b">
+        <v>0</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="O24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S24" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S24" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
     </row>
     <row r="25" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="3">
-        <v>0</v>
-      </c>
-      <c r="F25" s="3">
+        <v>12</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
         <v>10</v>
       </c>
-      <c r="G25" s="5" t="b">
+      <c r="G25" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -2088,48 +2707,48 @@
     </row>
     <row r="26" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>60</v>
+        <v>129</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="3">
+        <v>12</v>
+      </c>
+      <c r="E26" s="4">
+        <v>9</v>
+      </c>
+      <c r="F26" s="4">
         <v>11</v>
       </c>
-      <c r="F26" s="3">
-        <v>12</v>
-      </c>
-      <c r="G26" s="5" t="b">
-        <v>0</v>
+      <c r="G26" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1" t="s">
-        <v>62</v>
+        <v>138</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>71</v>
+        <v>140</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>72</v>
+        <v>141</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>73</v>
+        <v>142</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>74</v>
+        <v>143</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
@@ -2139,48 +2758,48 @@
     </row>
     <row r="27" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="3">
+        <v>12</v>
+      </c>
+      <c r="E27" s="4">
         <v>11</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="4">
         <v>13</v>
       </c>
-      <c r="G27" s="5" t="b">
+      <c r="G27" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
@@ -2190,175 +2809,175 @@
     </row>
     <row r="28" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>34</v>
+        <v>130</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="3">
-        <v>11</v>
-      </c>
-      <c r="F28" s="3">
+        <v>12</v>
+      </c>
+      <c r="E28" s="4">
+        <v>12</v>
+      </c>
+      <c r="F28" s="4">
         <v>15</v>
       </c>
-      <c r="G28" s="5" t="b">
-        <v>0</v>
+      <c r="G28" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>98</v>
+        <v>151</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>99</v>
+        <v>152</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>100</v>
+        <v>153</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>101</v>
+        <v>154</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>102</v>
+        <v>155</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>103</v>
+        <v>156</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>104</v>
+        <v>157</v>
       </c>
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
     </row>
     <row r="29" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="3">
-        <v>12</v>
-      </c>
-      <c r="F29" s="3">
+        <v>12</v>
+      </c>
+      <c r="E29" s="4">
+        <v>12</v>
+      </c>
+      <c r="F29" s="4">
         <v>17</v>
       </c>
-      <c r="G29" s="5" t="b">
+      <c r="G29" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="S29" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="U29" s="1"/>
     </row>
     <row r="30" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="3">
-        <v>12</v>
-      </c>
-      <c r="F30" s="3">
+        <v>12</v>
+      </c>
+      <c r="E30" s="4">
+        <v>12</v>
+      </c>
+      <c r="F30" s="4">
         <v>18</v>
       </c>
-      <c r="G30" s="5" t="b">
+      <c r="G30" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
     </row>
     <row r="31" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="3">
+        <v>12</v>
+      </c>
+      <c r="E31" s="4">
         <v>17</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="4">
         <v>30</v>
       </c>
-      <c r="G31" s="5" t="b">
+      <c r="G31" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H31" s="1"/>
@@ -2366,54 +2985,54 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="T31" s="1" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="U31" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="3">
+        <v>12</v>
+      </c>
+      <c r="E32" s="4">
         <v>30</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="4">
         <v>34</v>
       </c>
-      <c r="G32" s="5" t="b">
+      <c r="G32" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H32" s="1"/>
@@ -2421,54 +3040,54 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="S32" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="T32" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="U32" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="3">
+        <v>12</v>
+      </c>
+      <c r="E33" s="4">
         <v>35</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33" s="4">
         <v>39</v>
       </c>
-      <c r="G33" s="5" t="b">
+      <c r="G33" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H33" s="1"/>
@@ -2476,54 +3095,54 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="S33" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="T33" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="U33" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="3">
+        <v>12</v>
+      </c>
+      <c r="E34" s="4">
         <v>40</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="4">
         <v>44</v>
       </c>
-      <c r="G34" s="5" t="b">
+      <c r="G34" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H34" s="1"/>
@@ -2531,54 +3150,54 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="S34" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="T34" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="U34" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="3">
+        <v>12</v>
+      </c>
+      <c r="E35" s="4">
         <v>45</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35" s="4">
         <v>49</v>
       </c>
-      <c r="G35" s="5" t="b">
+      <c r="G35" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H35" s="1"/>
@@ -2586,54 +3205,54 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="S35" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="T35" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="U35" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="3">
+        <v>12</v>
+      </c>
+      <c r="E36" s="4">
         <v>50</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="4">
         <v>54</v>
       </c>
-      <c r="G36" s="5" t="b">
+      <c r="G36" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H36" s="1"/>
@@ -2641,54 +3260,54 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="S36" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="T36" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="U36" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="3">
+        <v>12</v>
+      </c>
+      <c r="E37" s="4">
         <v>55</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37" s="4">
         <v>59</v>
       </c>
-      <c r="G37" s="5" t="b">
+      <c r="G37" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H37" s="1"/>
@@ -2696,54 +3315,54 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="S37" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="T37" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="U37" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="3">
+        <v>12</v>
+      </c>
+      <c r="E38" s="4">
         <v>60</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38" s="4">
         <v>64</v>
       </c>
-      <c r="G38" s="5" t="b">
+      <c r="G38" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H38" s="1"/>
@@ -2751,54 +3370,54 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="S38" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="T38" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="U38" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="3">
+        <v>12</v>
+      </c>
+      <c r="E39" s="4">
         <v>65</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39" s="4">
         <v>69</v>
       </c>
-      <c r="G39" s="5" t="b">
+      <c r="G39" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H39" s="1"/>
@@ -2806,54 +3425,54 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="S39" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="T39" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="U39" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="3">
+        <v>12</v>
+      </c>
+      <c r="E40" s="4">
         <v>70</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F40" s="4">
         <v>74</v>
       </c>
-      <c r="G40" s="5" t="b">
+      <c r="G40" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H40" s="1"/>
@@ -2861,54 +3480,54 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="S40" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="T40" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="U40" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41" s="3">
+        <v>12</v>
+      </c>
+      <c r="E41" s="4">
         <v>75</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F41" s="4">
         <v>79</v>
       </c>
-      <c r="G41" s="5" t="b">
+      <c r="G41" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H41" s="1"/>
@@ -2916,54 +3535,54 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="R41" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="S41" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="T41" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="U41" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E42" s="3">
+        <v>12</v>
+      </c>
+      <c r="E42" s="4">
         <v>80</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42" s="4">
         <v>999</v>
       </c>
-      <c r="G42" s="5" t="b">
+      <c r="G42" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H42" s="1"/>
@@ -2971,164 +3590,164 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="S42" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="T42" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="U42" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E43" s="3">
+        <v>12</v>
+      </c>
+      <c r="E43" s="4">
         <v>13</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F43" s="4">
         <v>17</v>
       </c>
-      <c r="G43" s="5" t="b">
+      <c r="G43" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="R43" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="S43" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="T43" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="U43" s="1"/>
     </row>
     <row r="44" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="3">
+        <v>12</v>
+      </c>
+      <c r="E44" s="4">
         <v>15</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F44" s="4">
         <v>20</v>
       </c>
-      <c r="G44" s="5" t="b">
-        <v>0</v>
+      <c r="G44" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="R44" s="1" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="S44" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="T44" s="1" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="U44" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="3">
+        <v>12</v>
+      </c>
+      <c r="E45" s="4">
         <v>15</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F45" s="4">
         <v>999</v>
       </c>
-      <c r="G45" s="5" t="b">
+      <c r="G45" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H45" s="1"/>
@@ -3136,97 +3755,97 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1" t="s">
-        <v>124</v>
+        <v>166</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>126</v>
+        <v>167</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>127</v>
+        <v>168</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>128</v>
+        <v>169</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>129</v>
+        <v>170</v>
       </c>
       <c r="R45" s="1" t="s">
-        <v>130</v>
+        <v>171</v>
       </c>
       <c r="S45" s="1" t="s">
-        <v>131</v>
+        <v>172</v>
       </c>
       <c r="T45" s="1" t="s">
-        <v>132</v>
+        <v>173</v>
       </c>
       <c r="U45" s="1" t="s">
-        <v>123</v>
+        <v>174</v>
       </c>
     </row>
     <row r="46" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="3">
-        <v>0</v>
-      </c>
-      <c r="F46" s="3">
+        <v>12</v>
+      </c>
+      <c r="E46" s="4">
+        <v>0</v>
+      </c>
+      <c r="F46" s="4">
         <v>999</v>
       </c>
-      <c r="G46" s="5" t="b">
-        <v>1</v>
+      <c r="G46" s="7" t="b">
+        <v>0</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="R46" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="S46" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="T46" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="U46" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed 80 85 Masters
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/agegroups/FHQ-AgeGroups_fr_CA.xlsx
+++ b/owlcms/src/main/resources/agegroups/FHQ-AgeGroups_fr_CA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\local\agegroups\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\agegroups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16D41ED-4602-4FF5-A713-38D41C9F5125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577EDE71-D438-44C4-9417-E768D64F44DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2745" yWindow="1065" windowWidth="21600" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6405" yWindow="2040" windowWidth="21600" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BW Categories" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="176">
   <si>
     <t>code</t>
   </si>
@@ -185,9 +185,6 @@
     <t>F999 is always used as the last category in an age group</t>
   </si>
   <si>
-    <t>F70+</t>
-  </si>
-  <si>
     <t>YTH</t>
   </si>
   <si>
@@ -218,12 +215,6 @@
     <t>M75</t>
   </si>
   <si>
-    <t>M80+</t>
-  </si>
-  <si>
-    <t>F80+</t>
-  </si>
-  <si>
     <t>F40 35</t>
   </si>
   <si>
@@ -546,6 +537,18 @@
   </si>
   <si>
     <t>M999 284</t>
+  </si>
+  <si>
+    <t>F80</t>
+  </si>
+  <si>
+    <t>F85</t>
+  </si>
+  <si>
+    <t>M85</t>
+  </si>
+  <si>
+    <t>M80</t>
   </si>
 </sst>
 </file>
@@ -1387,10 +1390,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:U46"/>
+  <dimension ref="A1:U47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44:E44"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1474,7 +1477,7 @@
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
@@ -1490,32 +1493,32 @@
         <v>11</v>
       </c>
       <c r="G3" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -1525,7 +1528,7 @@
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
@@ -1545,28 +1548,28 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="L4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -1576,7 +1579,7 @@
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
@@ -1592,33 +1595,33 @@
         <v>15</v>
       </c>
       <c r="G5" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="O5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -1680,7 +1683,7 @@
     </row>
     <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
@@ -1701,28 +1704,28 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -1731,7 +1734,7 @@
     </row>
     <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
@@ -1752,34 +1755,34 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="S8" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
@@ -2336,7 +2339,7 @@
     </row>
     <row r="19" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>66</v>
+        <v>172</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
@@ -2349,7 +2352,7 @@
         <v>80</v>
       </c>
       <c r="F19" s="4">
-        <v>999</v>
+        <v>84</v>
       </c>
       <c r="G19" s="7" t="b">
         <v>0</v>
@@ -2391,7 +2394,7 @@
     </row>
     <row r="20" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
@@ -2401,7 +2404,7 @@
         <v>30</v>
       </c>
       <c r="E20" s="4">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="F20" s="4">
         <v>999</v>
@@ -2446,11 +2449,11 @@
     </row>
     <row r="21" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>30</v>
@@ -2501,11 +2504,11 @@
     </row>
     <row r="22" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>30</v>
@@ -2522,34 +2525,34 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M22" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="N22" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="O22" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="P22" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N22" s="1" t="s">
+      <c r="Q22" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="O22" s="1" t="s">
+      <c r="R22" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="S22" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="Q22" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
@@ -2560,7 +2563,7 @@
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>30</v>
@@ -2577,45 +2580,45 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="M23" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="N23" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="O23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q23" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="R23" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="N23" s="1" t="s">
+      <c r="S23" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="S23" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
     </row>
     <row r="24" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>30</v>
@@ -2627,7 +2630,7 @@
         <v>999</v>
       </c>
       <c r="G24" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>29</v>
@@ -2707,7 +2710,7 @@
     </row>
     <row r="26" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
@@ -2723,32 +2726,32 @@
         <v>11</v>
       </c>
       <c r="G26" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L26" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="M26" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="N26" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="L26" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="O26" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
@@ -2758,7 +2761,7 @@
     </row>
     <row r="27" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
@@ -2778,28 +2781,28 @@
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="N27" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="O27" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="P27" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
@@ -2809,7 +2812,7 @@
     </row>
     <row r="28" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
@@ -2830,28 +2833,28 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="K28" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="N28" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="L28" s="1" t="s">
+      <c r="O28" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="P28" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="N28" s="1" t="s">
+      <c r="Q28" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
@@ -2912,7 +2915,7 @@
     </row>
     <row r="30" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
@@ -2934,35 +2937,35 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="N30" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="L30" s="1" t="s">
+      <c r="O30" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="P30" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="N30" s="1" t="s">
+      <c r="Q30" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="O30" s="1" t="s">
+      <c r="R30" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q30" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="R30" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
     </row>
     <row r="31" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
@@ -2985,39 +2988,39 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O31" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="M31" s="1" t="s">
+      <c r="P31" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="N31" s="1" t="s">
+      <c r="Q31" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="O31" s="1" t="s">
+      <c r="R31" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="P31" s="1" t="s">
+      <c r="S31" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="Q31" s="1" t="s">
+      <c r="T31" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="R31" s="1" t="s">
+      <c r="U31" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="S31" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="T31" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="U31" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
@@ -3237,7 +3240,7 @@
     </row>
     <row r="36" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
@@ -3347,7 +3350,7 @@
     </row>
     <row r="38" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
@@ -3402,7 +3405,7 @@
     </row>
     <row r="39" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
@@ -3457,7 +3460,7 @@
     </row>
     <row r="40" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
@@ -3512,7 +3515,7 @@
     </row>
     <row r="41" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
@@ -3567,7 +3570,7 @@
     </row>
     <row r="42" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>65</v>
+        <v>175</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
@@ -3580,7 +3583,7 @@
         <v>80</v>
       </c>
       <c r="F42" s="4">
-        <v>999</v>
+        <v>84</v>
       </c>
       <c r="G42" s="7" t="b">
         <v>0</v>
@@ -3622,20 +3625,20 @@
     </row>
     <row r="43" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>55</v>
+        <v>174</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E43" s="4">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="F43" s="4">
-        <v>17</v>
+        <v>999</v>
       </c>
       <c r="G43" s="7" t="b">
         <v>0</v>
@@ -3643,9 +3646,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
-      <c r="K43" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="K43" s="1"/>
       <c r="L43" s="1" t="s">
         <v>18</v>
       </c>
@@ -3671,72 +3672,74 @@
         <v>25</v>
       </c>
       <c r="T43" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U43" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U43" s="1"/>
     </row>
     <row r="44" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E44" s="4">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F44" s="4">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G44" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
+      <c r="K44" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="L44" s="1" t="s">
-        <v>83</v>
+        <v>18</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="R44" s="1" t="s">
-        <v>89</v>
+        <v>24</v>
       </c>
       <c r="S44" s="1" t="s">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="T44" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="U44" s="1" t="s">
-        <v>92</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="U44" s="1"/>
     </row>
     <row r="45" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>12</v>
@@ -3745,7 +3748,7 @@
         <v>15</v>
       </c>
       <c r="F45" s="4">
-        <v>999</v>
+        <v>20</v>
       </c>
       <c r="G45" s="7" t="b">
         <v>0</v>
@@ -3755,49 +3758,49 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1" t="s">
-        <v>166</v>
+        <v>80</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>167</v>
+        <v>82</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>168</v>
+        <v>83</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>169</v>
+        <v>84</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>170</v>
+        <v>85</v>
       </c>
       <c r="R45" s="1" t="s">
-        <v>171</v>
+        <v>86</v>
       </c>
       <c r="S45" s="1" t="s">
-        <v>172</v>
+        <v>87</v>
       </c>
       <c r="T45" s="1" t="s">
-        <v>173</v>
+        <v>88</v>
       </c>
       <c r="U45" s="1" t="s">
-        <v>174</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>128</v>
+        <v>45</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E46" s="4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F46" s="4">
         <v>999</v>
@@ -3805,46 +3808,101 @@
       <c r="G46" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q46" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R46" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="S46" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="T46" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="U46" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="4">
+        <v>0</v>
+      </c>
+      <c r="F47" s="4">
+        <v>999</v>
+      </c>
+      <c r="G47" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="1" t="s">
+      <c r="I47" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J46" s="1" t="s">
+      <c r="J47" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K46" s="1" t="s">
+      <c r="K47" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L46" s="1" t="s">
+      <c r="L47" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M46" s="1" t="s">
+      <c r="M47" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N46" s="1" t="s">
+      <c r="N47" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O46" s="1" t="s">
+      <c r="O47" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P46" s="1" t="s">
+      <c r="P47" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q46" s="1" t="s">
+      <c r="Q47" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R46" s="1" t="s">
+      <c r="R47" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="S46" s="1" t="s">
+      <c r="S47" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="T46" s="1" t="s">
+      <c r="T47" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U46" s="1" t="s">
+      <c r="U47" s="1" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>